<commit_message>
extrude and move changes
</commit_message>
<xml_diff>
--- a/Timeline Gannt.xlsx
+++ b/Timeline Gannt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parth\Documents\GENE\GENE121-Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C8AC73-C493-4D7A-89ED-A84787F24C07}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0708D715-A8A2-4379-B0C5-3258C2A91B3B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{55E1E339-1649-664C-9BC8-CF661C217C26}"/>
   </bookViews>
@@ -75,6 +75,12 @@
     <t>Servo code</t>
   </si>
   <si>
+    <t>pen movment</t>
+  </si>
+  <si>
+    <t>print movement</t>
+  </si>
+  <si>
     <t>"Gcode" read in</t>
   </si>
   <si>
@@ -103,12 +109,6 @@
   </si>
   <si>
     <t>mount for base</t>
-  </si>
-  <si>
-    <t>Pen movment</t>
-  </si>
-  <si>
-    <t>Print movement</t>
   </si>
 </sst>
 </file>
@@ -205,6 +205,61 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Pre-Sprint</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -213,8 +268,82 @@
         <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Start Date</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$4:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Mockups </c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3D pen testing</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kinematic measurments</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>43389</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43389</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43389</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-BA33-4415-85E8-40E5C5C2FB72}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="1"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Duration</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent2"/>
@@ -244,25 +373,25 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$4:$D$6</c:f>
+              <c:f>Sheet1!$C$4:$C$6</c:f>
               <c:numCache>
-                <c:formatCode>d\-mmm</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>43393</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43390</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43390</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-BA33-4415-85E8-40E5C5C2FB72}"/>
+              <c16:uniqueId val="{00000005-BA33-4415-85E8-40E5C5C2FB72}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -274,7 +403,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="55"/>
         <c:overlap val="100"/>
         <c:axId val="402010680"/>
         <c:axId val="402013632"/>
@@ -394,6 +523,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -472,14 +632,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-CA"/>
               <a:t>Sprint</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-CA" baseline="0"/>
               <a:t> 1</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CA"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -520,15 +680,132 @@
         <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$9</c:f>
+              <c:f>Sheet1!$B$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>End Date</c:v>
+                  <c:v>Start Date</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$10:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>CAD for rack and pinion</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3D modelling</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Laser printing</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>z axis build</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>x,y axis build</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>mount for base</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Colour scan</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Servo code</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Motor base movment</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Kinematic calculations</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Testing</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Full testing:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>43407</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43408</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43410</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43408</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43407</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43412</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43411</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43412</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43410</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43408</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43411</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43413</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-536F-4766-9FE3-9E5B2E2245EE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Duration</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -549,10 +826,10 @@
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>CAD for rack and pinion</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>3D modelling</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>CAD for rack and pinion</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Laser printing</c:v>
@@ -589,52 +866,52 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$10:$D$21</c:f>
+              <c:f>Sheet1!$C$10:$C$21</c:f>
               <c:numCache>
-                <c:formatCode>d\-mmm</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>43412</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43412</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43412</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43411</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43410</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43413</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43412</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43413</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43412</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43410</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43412</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43413</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-536F-4766-9FE3-9E5B2E2245EE}"/>
+              <c16:uniqueId val="{00000003-536F-4766-9FE3-9E5B2E2245EE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -646,7 +923,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="55"/>
         <c:overlap val="100"/>
         <c:axId val="405993304"/>
         <c:axId val="405997240"/>
@@ -654,7 +931,7 @@
       <c:catAx>
         <c:axId val="405993304"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -708,7 +985,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -766,6 +1043,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -825,6 +1133,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Sprint 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -862,15 +1195,102 @@
         <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$26</c:f>
+              <c:f>Sheet1!$B$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>End Date</c:v>
+                  <c:v>Start Date</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$27:$A$33</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Build height</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Neighbour sensitivity code</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>pen movment</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>print movement</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Main</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>"Gcode" read in</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Full testing:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$27:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>43416</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43418</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43416</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43416</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43418</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43416</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43420</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2D6A-43BD-89B9-87AC777D9075}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Duration</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -897,10 +1317,10 @@
                   <c:v>Neighbour sensitivity code</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Pen movment</c:v>
+                  <c:v>pen movment</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Print movement</c:v>
+                  <c:v>print movement</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Main</c:v>
@@ -916,37 +1336,37 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$27:$D$33</c:f>
+              <c:f>Sheet1!$C$27:$C$33</c:f>
               <c:numCache>
-                <c:formatCode>d\-mmm</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>43418</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43420</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43417</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43421</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43420</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43418</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43423</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-5E36-4C46-BBD7-92D40F5586D9}"/>
+              <c16:uniqueId val="{00000001-2D6A-43BD-89B9-87AC777D9075}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -958,15 +1378,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
+        <c:gapWidth val="55"/>
         <c:overlap val="100"/>
-        <c:axId val="526939328"/>
-        <c:axId val="526940640"/>
+        <c:axId val="521649376"/>
+        <c:axId val="521652984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="526939328"/>
+        <c:axId val="521649376"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1007,7 +1427,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="526940640"/>
+        <c:crossAx val="521652984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1015,12 +1435,12 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="526940640"/>
+        <c:axId val="521652984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1066,7 +1486,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="526939328"/>
+        <c:crossAx val="521649376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1078,6 +1498,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -2803,8 +3254,8 @@
       <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>217170</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>693420</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
@@ -2834,22 +3285,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>791817</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>59635</xdr:rowOff>
+      <xdr:colOff>783739</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>193189</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>235226</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>6626</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>708212</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>148366</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D059705-E36F-4070-84F1-DB0B72065A1C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB9FDC7B-7E6F-497F-95D7-A2664362F54E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3169,8 +3620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF1DAEA-7BA0-6D47-B1D7-56EA6307BD6D}">
   <dimension ref="A2:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3260,13 +3711,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="3">
-        <v>43408</v>
+        <v>43407</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10" s="3">
         <v>43412</v>
@@ -3274,13 +3725,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3">
-        <v>43407</v>
+        <v>43408</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="3">
         <v>43412</v>
@@ -3330,7 +3781,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B15" s="6">
         <v>43412</v>
@@ -3372,7 +3823,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B18" s="3">
         <v>43410</v>
@@ -3386,7 +3837,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B19" s="3">
         <v>43408</v>
@@ -3400,7 +3851,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B20" s="6">
         <v>43411</v>
@@ -3414,7 +3865,7 @@
     </row>
     <row r="21" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B21" s="8">
         <v>43413</v>
@@ -3429,7 +3880,7 @@
     <row r="22" spans="1:4" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -3448,7 +3899,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B27" s="3">
         <v>43416</v>
@@ -3462,7 +3913,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B28" s="3">
         <v>43418</v>
@@ -3476,7 +3927,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B29" s="3">
         <v>43416</v>
@@ -3490,7 +3941,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B30" s="3">
         <v>43416</v>
@@ -3504,7 +3955,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B31" s="3">
         <v>43418</v>
@@ -3518,7 +3969,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B32" s="3">
         <v>43416</v>
@@ -3532,7 +3983,7 @@
     </row>
     <row r="33" spans="1:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B33" s="8">
         <v>43420</v>

</xml_diff>